<commit_message>
Prouct excel sheet added
</commit_message>
<xml_diff>
--- a/Vtiger_Framework/Test Data/ExcelData/TestData Vtiger.xlsx
+++ b/Vtiger_Framework/Test Data/ExcelData/TestData Vtiger.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\Csharp Study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioRepos\Vtiger_Framework\Vtiger_Framework\Test Data\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14C6F45-17C0-4AB6-A91A-ABBA8AB2692A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B7A6C2-9FA9-4781-AF5A-7FE9A690DCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="product" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>admin</t>
   </si>
@@ -37,6 +38,33 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>productname</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>commissionrate</t>
+  </si>
+  <si>
+    <t>unitqty</t>
+  </si>
+  <si>
+    <t>stockquantity</t>
+  </si>
+  <si>
+    <t>Ikegai</t>
+  </si>
+  <si>
+    <t>Mindset</t>
+  </si>
+  <si>
+    <t>Rich Dad poor Dad</t>
+  </si>
+  <si>
+    <t>Atomic Habbits</t>
   </si>
 </sst>
 </file>
@@ -52,12 +80,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -397,4 +432,160 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A928597-9CF2-4BF7-9478-D7929B36AEEB}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>120</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>160</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>